<commit_message>
Updated find_empty_date_column added find added name based check in added number ID based check in
</commit_message>
<xml_diff>
--- a/ATT.xlsx
+++ b/ATT.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:workbookPr codeName="ThisWorkbook"/>
-  <s:bookViews>
-    <s:workbookView activeTab="0"/>
-  </s:bookViews>
-  <s:sheets>
-    <s:sheet name="Attendance" sheetId="1" r:id="rId1"/>
-    <s:sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <s:sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-  </s:sheets>
-  <s:definedNames/>
-  <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
-</s:workbook>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="510" yWindow="615" windowWidth="13095" windowHeight="6855"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Attendance" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+  </sheets>
+  <calcPr calcId="125725"/>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Number</t>
   </si>
@@ -31,25 +31,30 @@
   </si>
   <si>
     <t>July 17 2016</t>
+  </si>
+  <si>
+    <t>07:53 PM</t>
+  </si>
+  <si>
+    <t>JJ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -65,16 +70,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -362,23 +367,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="4" min="4" width="11.28515625"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -395,43 +396,47 @@
         <v>4</v>
       </c>
     </row>
+    <row r="2" spans="1:5">
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added payment approval and member addition
</commit_message>
<xml_diff>
--- a/ATT.xlsx
+++ b/ATT.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <bookViews>
-    <workbookView xWindow="510" yWindow="615" windowWidth="13095" windowHeight="6855"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Attendance" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-  </sheets>
-  <calcPr calcId="125725"/>
-</workbook>
+<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <s:workbookPr codeName="ThisWorkbook"/>
+  <s:bookViews>
+    <s:workbookView activeTab="0"/>
+  </s:bookViews>
+  <s:sheets>
+    <s:sheet name="Attendance" sheetId="1" r:id="rId1"/>
+    <s:sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <s:sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+  </s:sheets>
+  <s:definedNames/>
+  <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
+</s:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
   <si>
     <t>Number</t>
   </si>
@@ -33,28 +33,35 @@
     <t>July 17 2016</t>
   </si>
   <si>
+    <t>xc</t>
+  </si>
+  <si>
+    <t>PAID</t>
+  </si>
+  <si>
     <t>07:53 PM</t>
   </si>
   <si>
-    <t>JJ</t>
+    <t>js</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -70,16 +77,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -367,16 +374,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" width="11.28515625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -397,46 +408,73 @@
       </c>
     </row>
     <row r="2" spans="1:5">
+      <c r="A2" t="n">
+        <v>9</v>
+      </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3">
+      <c r="A3" t="n">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="n">
+        <v>99</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed name_check_in and number_check_in
</commit_message>
<xml_diff>
--- a/ATT.xlsx
+++ b/ATT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
   <si>
     <t>Number</t>
   </si>
@@ -33,6 +33,9 @@
     <t>July 17 2016</t>
   </si>
   <si>
+    <t>July 18 2016</t>
+  </si>
+  <si>
     <t>xc</t>
   </si>
   <si>
@@ -42,7 +45,13 @@
     <t>07:53 PM</t>
   </si>
   <si>
+    <t>02:34 PM</t>
+  </si>
+  <si>
     <t>js</t>
+  </si>
+  <si>
+    <t>ccff</t>
   </si>
 </sst>
 </file>
@@ -379,7 +388,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -390,7 +399,7 @@
     <col bestFit="1" customWidth="1" max="4" min="4" width="11.28515625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -406,38 +415,54 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" t="n">
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3" t="n">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4" t="n">
         <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5"/>
+    <row r="5" spans="1:6">
+      <c r="A5" t="n">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
incoreperated tkinter interface with excel work
</commit_message>
<xml_diff>
--- a/ATT.xlsx
+++ b/ATT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
   <si>
     <t>Number</t>
   </si>
@@ -36,6 +36,9 @@
     <t>July 18 2016</t>
   </si>
   <si>
+    <t>July 28 2016</t>
+  </si>
+  <si>
     <t>xc</t>
   </si>
   <si>
@@ -46,6 +49,9 @@
   </si>
   <si>
     <t>02:34 PM</t>
+  </si>
+  <si>
+    <t>03:31 PM</t>
   </si>
   <si>
     <t>js</t>
@@ -388,10 +394,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -399,7 +405,7 @@
     <col bestFit="1" customWidth="1" max="4" min="4" width="11.28515625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -418,48 +424,57 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" t="n">
+        <v>123456789</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="n">
+        <v>246812468</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="n">
+        <v>789564123</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="n">
-        <v>99</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="A5" t="n">
-        <v>0</v>
+        <v>258147369</v>
       </c>
       <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Name Check In GUI
</commit_message>
<xml_diff>
--- a/ATT.xlsx
+++ b/ATT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
   <si>
     <t>Number</t>
   </si>
@@ -39,6 +39,9 @@
     <t>July 28 2016</t>
   </si>
   <si>
+    <t>July 29 2016</t>
+  </si>
+  <si>
     <t>xc</t>
   </si>
   <si>
@@ -54,10 +57,13 @@
     <t>03:31 PM</t>
   </si>
   <si>
-    <t>js</t>
-  </si>
-  <si>
-    <t>ccff</t>
+    <t>11:05 AM</t>
+  </si>
+  <si>
+    <t>j s</t>
+  </si>
+  <si>
+    <t>11:17 AM</t>
   </si>
 </sst>
 </file>
@@ -394,10 +400,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -405,7 +411,7 @@
     <col bestFit="1" customWidth="1" max="4" min="4" width="11.28515625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -427,59 +433,47 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" t="n">
         <v>123456789</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="A3" t="n">
-        <v>246812468</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="n">
-        <v>789564123</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="n">
-        <v>258147369</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" t="s">
-        <v>11</v>
+        <v>246810120</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added member addition GUI
</commit_message>
<xml_diff>
--- a/ATT.xlsx
+++ b/ATT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
   <si>
     <t>Number</t>
   </si>
@@ -42,7 +42,7 @@
     <t>July 29 2016</t>
   </si>
   <si>
-    <t>xc</t>
+    <t>x c</t>
   </si>
   <si>
     <t>PAID</t>
@@ -64,6 +64,24 @@
   </si>
   <si>
     <t>11:17 AM</t>
+  </si>
+  <si>
+    <t>monty python</t>
+  </si>
+  <si>
+    <t>12:35 PM</t>
+  </si>
+  <si>
+    <t>safe way</t>
+  </si>
+  <si>
+    <t>12:36 PM</t>
+  </si>
+  <si>
+    <t>taylormans</t>
+  </si>
+  <si>
+    <t>12:48 PM</t>
   </si>
 </sst>
 </file>
@@ -400,10 +418,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -471,6 +489,40 @@
         <v>15</v>
       </c>
     </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="n">
+        <v>135693201</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="n">
+        <v>789456321</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="n">
+        <v>102450690</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8"/>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Updated member addition GUI
</commit_message>
<xml_diff>
--- a/ATT.xlsx
+++ b/ATT.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:workbookPr codeName="ThisWorkbook"/>
-  <s:bookViews>
-    <s:workbookView activeTab="0"/>
-  </s:bookViews>
-  <s:sheets>
-    <s:sheet name="Attendance" sheetId="1" r:id="rId1"/>
-    <s:sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <s:sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-  </s:sheets>
-  <s:definedNames/>
-  <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
-</s:workbook>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="390" yWindow="825" windowWidth="18615" windowHeight="10905"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Attendance" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+  </sheets>
+  <calcPr calcId="125725"/>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Number</t>
   </si>
@@ -58,49 +58,27 @@
   </si>
   <si>
     <t>11:05 AM</t>
-  </si>
-  <si>
-    <t>j s</t>
-  </si>
-  <si>
-    <t>11:17 AM</t>
-  </si>
-  <si>
-    <t>monty python</t>
-  </si>
-  <si>
-    <t>12:35 PM</t>
-  </si>
-  <si>
-    <t>safe way</t>
-  </si>
-  <si>
-    <t>12:36 PM</t>
-  </si>
-  <si>
-    <t>taylormans</t>
-  </si>
-  <si>
-    <t>12:48 PM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="000000000"/>
+  </numFmts>
   <fonts count="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -116,16 +94,19 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -413,24 +394,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="4" min="4" width="11.28515625"/>
+    <col min="1" max="1" width="11.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -456,7 +435,7 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" t="n">
+      <c r="A2" s="3">
         <v>123456789</v>
       </c>
       <c r="B2" t="s">
@@ -479,88 +458,59 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" t="n">
-        <v>246810120</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s">
-        <v>15</v>
-      </c>
+      <c r="A3" s="3"/>
+      <c r="B3"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" t="n">
-        <v>135693201</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" t="s">
-        <v>17</v>
-      </c>
+      <c r="A4" s="3"/>
+      <c r="B4"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" t="n">
-        <v>789456321</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" t="s">
-        <v>19</v>
-      </c>
+      <c r="A5" s="3"/>
+      <c r="B5"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" t="n">
-        <v>102450690</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8"/>
+      <c r="A6" s="3"/>
+      <c r="B6"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="3"/>
+      <c r="B7"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="3"/>
+      <c r="B8"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="3"/>
+      <c r="B9"/>
+    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
listbox shows members that have signed in
</commit_message>
<xml_diff>
--- a/ATT.xlsx
+++ b/ATT.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <bookViews>
-    <workbookView xWindow="390" yWindow="825" windowWidth="18615" windowHeight="10905"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Attendance" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-  </sheets>
-  <calcPr calcId="125725"/>
-</workbook>
+<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <s:workbookPr codeName="ThisWorkbook"/>
+  <s:bookViews>
+    <s:workbookView activeTab="0"/>
+  </s:bookViews>
+  <s:sheets>
+    <s:sheet name="Attendance" sheetId="1" r:id="rId1"/>
+    <s:sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <s:sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+  </s:sheets>
+  <s:definedNames/>
+  <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
+</s:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
   <si>
     <t>Number</t>
   </si>
@@ -42,6 +42,9 @@
     <t>July 29 2016</t>
   </si>
   <si>
+    <t>July 30 2016</t>
+  </si>
+  <si>
     <t>x c</t>
   </si>
   <si>
@@ -58,6 +61,21 @@
   </si>
   <si>
     <t>11:05 AM</t>
+  </si>
+  <si>
+    <t>04:16 PM</t>
+  </si>
+  <si>
+    <t>coo cuu</t>
+  </si>
+  <si>
+    <t>04:53 PM</t>
+  </si>
+  <si>
+    <t>koo case</t>
+  </si>
+  <si>
+    <t>06:38 PM</t>
   </si>
 </sst>
 </file>
@@ -65,20 +83,20 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="000000000"/>
+    <numFmt formatCode="000000000" numFmtId="164"/>
   </numFmts>
   <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -94,19 +112,19 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -394,21 +412,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col customWidth="1" max="1" min="1" style="2" width="11.42578125"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" style="1" width="13.85546875"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" style="1" width="11.28515625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -433,84 +455,111 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="3">
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="3" t="n">
         <v>123456789</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="3"/>
-      <c r="B3"/>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="3"/>
-      <c r="B4"/>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="3"/>
-      <c r="B5"/>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="3"/>
-      <c r="B6"/>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="3"/>
-      <c r="B7"/>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="3"/>
-      <c r="B8"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="3"/>
-      <c r="B9"/>
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="3" t="n">
+        <v>796448521</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="3" t="n">
+        <v>312456787</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="3" t="n"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="3" t="n"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="3" t="n"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="3" t="n"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="3" t="n"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Force user to enter valid first and last name along with a valid number (natural number).
</commit_message>
<xml_diff>
--- a/ATT.xlsx
+++ b/ATT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="45">
   <si>
     <t>Number</t>
   </si>
@@ -84,6 +84,9 @@
     <t>August 04 2016</t>
   </si>
   <si>
+    <t>August 06 2016</t>
+  </si>
+  <si>
     <t>monty python</t>
   </si>
   <si>
@@ -142,6 +145,12 @@
   </si>
   <si>
     <t>ruby perl</t>
+  </si>
+  <si>
+    <t>assad</t>
+  </si>
+  <si>
+    <t>sajdsadasd</t>
   </si>
 </sst>
 </file>
@@ -484,7 +493,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V9"/>
+  <dimension ref="A1:W9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
       <selection activeCell="U10" sqref="U10"/>
@@ -498,7 +507,7 @@
     <col bestFit="1" customWidth="1" max="10" min="10" style="1" width="14.140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:23">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -565,16 +574,19 @@
       <c r="V1" t="s">
         <v>21</v>
       </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:23">
       <c r="A2" s="3" t="n">
         <v>123456789</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D2" s="4" t="n">
         <v>0.411805555555556</v>
@@ -610,36 +622,36 @@
         <v>0.8284722222222222</v>
       </c>
       <c r="O2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="Q2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="R2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="S2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="T2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="U2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="V2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:23">
       <c r="A3" s="3" t="n">
         <v>796448521</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D3" s="4" t="n">
         <v>0.411805555555556</v>
@@ -675,27 +687,27 @@
         <v>0.536805555555556</v>
       </c>
       <c r="Q3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="T3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:23">
       <c r="A4" s="3" t="n">
         <v>312456787</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D4" s="4" t="n">
         <v>0.411805555555556</v>
@@ -731,19 +743,19 @@
         <v>0.536805555555556</v>
       </c>
       <c r="Q4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="S4" s="4" t="n">
         <v>0.536805555555556</v>
       </c>
       <c r="U4" s="4" t="n"/>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:23">
       <c r="A5" s="3" t="n">
         <v>875412639</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D5" s="4" t="n">
         <v>0.536805555555556</v>
@@ -767,24 +779,34 @@
         <v>0.536805555555556</v>
       </c>
       <c r="S5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:23">
       <c r="A6" s="3" t="n">
         <v>741852963</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:22">
-      <c r="A7" s="3" t="n"/>
+    <row r="7" spans="1:23">
+      <c r="A7" s="3" t="n">
+        <v>232</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="8" spans="1:22">
-      <c r="A8" s="3" t="n"/>
+    <row r="8" spans="1:23">
+      <c r="A8" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:23">
       <c r="A9" s="3" t="n"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GUI for editing member information
</commit_message>
<xml_diff>
--- a/ATT.xlsx
+++ b/ATT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="53">
   <si>
     <t>Number</t>
   </si>
@@ -24,9 +24,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Paid</t>
-  </si>
-  <si>
     <t>July 5 2016</t>
   </si>
   <si>
@@ -87,70 +84,97 @@
     <t>August 06 2016</t>
   </si>
   <si>
+    <t>August 08 2016</t>
+  </si>
+  <si>
+    <t>August 09 2016</t>
+  </si>
+  <si>
+    <t>monty's pythons</t>
+  </si>
+  <si>
+    <t>02:34 PM</t>
+  </si>
+  <si>
+    <t>03:31 PM</t>
+  </si>
+  <si>
+    <t>11:05 AM</t>
+  </si>
+  <si>
+    <t>04:16 PM</t>
+  </si>
+  <si>
+    <t>06:42 PM</t>
+  </si>
+  <si>
+    <t>03:58 PM</t>
+  </si>
+  <si>
+    <t>06:26 PM</t>
+  </si>
+  <si>
+    <t>09:59 PM</t>
+  </si>
+  <si>
+    <t>03:56 PM</t>
+  </si>
+  <si>
+    <t>02:44 PM</t>
+  </si>
+  <si>
+    <t>java scripter</t>
+  </si>
+  <si>
+    <t>04:53 PM</t>
+  </si>
+  <si>
+    <t>06:15 PM</t>
+  </si>
+  <si>
+    <t>06:44 PM</t>
+  </si>
+  <si>
+    <t>03:59 PM</t>
+  </si>
+  <si>
+    <t>03:57 PM</t>
+  </si>
+  <si>
+    <t>darkest coffees</t>
+  </si>
+  <si>
+    <t>06:38 PM</t>
+  </si>
+  <si>
+    <t>name nom</t>
+  </si>
+  <si>
+    <t>ruby perl</t>
+  </si>
+  <si>
+    <t>x code</t>
+  </si>
+  <si>
+    <t>php node</t>
+  </si>
+  <si>
+    <t>02:45 PM</t>
+  </si>
+  <si>
+    <t>java script</t>
+  </si>
+  <si>
+    <t>PAID</t>
+  </si>
+  <si>
     <t>monty python</t>
   </si>
   <si>
-    <t>PAID</t>
-  </si>
-  <si>
-    <t>02:34 PM</t>
-  </si>
-  <si>
-    <t>03:31 PM</t>
-  </si>
-  <si>
-    <t>11:05 AM</t>
-  </si>
-  <si>
-    <t>04:16 PM</t>
-  </si>
-  <si>
-    <t>06:42 PM</t>
-  </si>
-  <si>
-    <t>03:58 PM</t>
-  </si>
-  <si>
-    <t>06:26 PM</t>
-  </si>
-  <si>
-    <t>09:59 PM</t>
-  </si>
-  <si>
-    <t>java scriptss</t>
-  </si>
-  <si>
-    <t>04:53 PM</t>
-  </si>
-  <si>
-    <t>06:15 PM</t>
-  </si>
-  <si>
-    <t>06:44 PM</t>
-  </si>
-  <si>
-    <t>03:59 PM</t>
-  </si>
-  <si>
-    <t>darkest coffee</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>06:38 PM</t>
-  </si>
-  <si>
-    <t>name nom</t>
-  </si>
-  <si>
-    <t>ruby perl</t>
-  </si>
-  <si>
-    <t>assad</t>
-  </si>
-  <si>
-    <t>sajdsadasd</t>
+    <t>d code</t>
+  </si>
+  <si>
+    <t>turtwig overgrow</t>
   </si>
 </sst>
 </file>
@@ -493,100 +517,101 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W10"/>
+  <dimension ref="A1:Y9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="U10" sqref="U10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0" zoomScale="48" zoomScaleNormal="48">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col customWidth="1" max="1" min="1" style="2" width="11.42578125"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" style="1" width="13.85546875"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" style="1" width="15.7109375"/>
     <col bestFit="1" customWidth="1" max="4" min="4" style="1" width="11.28515625"/>
     <col bestFit="1" customWidth="1" max="10" min="10" style="1" width="14.140625"/>
+    <col bestFit="1" customWidth="1" max="23" min="23" style="1" width="14.140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>22</v>
       </c>
+      <c r="Y1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:25">
       <c r="A2" s="3" t="n">
         <v>123456789</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="D2" s="4" t="n">
         <v>0.411805555555556</v>
@@ -645,13 +670,22 @@
       <c r="V2" t="s">
         <v>32</v>
       </c>
+      <c r="X2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:25">
       <c r="A3" s="3" t="n">
         <v>796448521</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>48</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
       </c>
       <c r="D3" s="4" t="n">
         <v>0.411805555555556</v>
@@ -687,27 +721,30 @@
         <v>0.536805555555556</v>
       </c>
       <c r="Q3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="R3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="S3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="T3" t="s">
-        <v>37</v>
+        <v>39</v>
+      </c>
+      <c r="X3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:25">
       <c r="A4" s="3" t="n">
-        <v>312456787</v>
+        <v>543543543</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D4" s="4" t="n">
         <v>0.411805555555556</v>
@@ -743,19 +780,19 @@
         <v>0.536805555555556</v>
       </c>
       <c r="Q4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="S4" s="4" t="n">
         <v>0.536805555555556</v>
       </c>
       <c r="U4" s="4" t="n"/>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:25">
       <c r="A5" s="3" t="n">
         <v>875412639</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D5" s="4" t="n">
         <v>0.536805555555556</v>
@@ -779,37 +816,45 @@
         <v>0.536805555555556</v>
       </c>
       <c r="S5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:23">
+    <row r="6" spans="1:25">
       <c r="A6" s="3" t="n">
         <v>741852963</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="X6" t="s">
+        <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:25">
       <c r="A7" s="3" t="n">
-        <v>232</v>
+        <v>604604604</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>51</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:25">
       <c r="A8" s="3" t="n">
-        <v>1</v>
+        <v>789789789</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>52</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:25">
       <c r="A9" s="3" t="n"/>
     </row>
-    <row r="10" spans="1:23"/>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Fixed auto focus selection details on multiple names.
</commit_message>
<xml_diff>
--- a/ATT.xlsx
+++ b/ATT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="61">
   <si>
     <t>Number</t>
   </si>
@@ -177,25 +177,28 @@
     <t>sql database</t>
   </si>
   <si>
+    <t>03:52 PM</t>
+  </si>
+  <si>
     <t>node .js</t>
   </si>
   <si>
     <t>05:53 PM</t>
   </si>
   <si>
-    <t>02:43 PM</t>
-  </si>
-  <si>
     <t>a d</t>
   </si>
   <si>
-    <t>02:45 PM</t>
-  </si>
-  <si>
-    <t>darkest coffee</t>
-  </si>
-  <si>
-    <t>02:53 PM</t>
+    <t>03:05 PM</t>
+  </si>
+  <si>
+    <t>03:53 PM</t>
+  </si>
+  <si>
+    <t>x codes</t>
+  </si>
+  <si>
+    <t>monty's pythons</t>
   </si>
 </sst>
 </file>
@@ -540,8 +543,8 @@
   </sheetPr>
   <dimension ref="A1:AB10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0" zoomScale="115" zoomScaleNormal="115">
-      <selection activeCell="AB2" sqref="AB2:AB10"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0" zoomScale="115" zoomScaleNormal="115">
+      <selection activeCell="AB10" sqref="AB2:AB10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -645,7 +648,7 @@
         <v>123456789</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
         <v>29</v>
@@ -720,7 +723,7 @@
         <v>41</v>
       </c>
       <c r="AB2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:28">
@@ -728,7 +731,7 @@
         <v>543543543</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="D3" s="4" t="n">
         <v>0.411805555555556</v>
@@ -770,9 +773,6 @@
         <v>0.536805555555556</v>
       </c>
       <c r="U3" s="4" t="n"/>
-      <c r="AB3" t="s">
-        <v>57</v>
-      </c>
     </row>
     <row r="4" spans="1:28">
       <c r="A4" s="3" t="n">
@@ -808,9 +808,6 @@
       <c r="S4" t="s">
         <v>45</v>
       </c>
-      <c r="AB4" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="5" spans="1:28">
       <c r="A5" s="3" t="n">
@@ -831,7 +828,7 @@
         <v>604604604</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="C6" t="s">
         <v>29</v>
@@ -849,7 +846,7 @@
         <v>50</v>
       </c>
       <c r="AB6" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:28">
@@ -862,9 +859,6 @@
       <c r="X7" t="s">
         <v>39</v>
       </c>
-      <c r="AB7" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="8" spans="1:28">
       <c r="A8" s="3" t="n">
@@ -877,7 +871,7 @@
         <v>41</v>
       </c>
       <c r="AB8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:28">
@@ -885,12 +879,9 @@
         <v>321321321</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="AA9" t="s">
-        <v>54</v>
-      </c>
-      <c r="AB9" t="s">
         <v>55</v>
       </c>
     </row>
@@ -903,6 +894,78 @@
       </c>
       <c r="C10" t="s">
         <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" t="s">
+        <v>57</v>
+      </c>
+      <c r="H10" t="s">
+        <v>57</v>
+      </c>
+      <c r="I10" t="s">
+        <v>57</v>
+      </c>
+      <c r="J10" t="s">
+        <v>57</v>
+      </c>
+      <c r="K10" t="s">
+        <v>57</v>
+      </c>
+      <c r="L10" t="s">
+        <v>57</v>
+      </c>
+      <c r="M10" t="s">
+        <v>57</v>
+      </c>
+      <c r="N10" t="s">
+        <v>57</v>
+      </c>
+      <c r="O10" t="s">
+        <v>57</v>
+      </c>
+      <c r="P10" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>57</v>
+      </c>
+      <c r="R10" t="s">
+        <v>57</v>
+      </c>
+      <c r="S10" t="s">
+        <v>57</v>
+      </c>
+      <c r="T10" t="s">
+        <v>57</v>
+      </c>
+      <c r="U10" t="s">
+        <v>57</v>
+      </c>
+      <c r="V10" t="s">
+        <v>57</v>
+      </c>
+      <c r="W10" t="s">
+        <v>57</v>
+      </c>
+      <c r="X10" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed text bug with editing member information interface where the "Last Name:" label was labeled as "First Name:". Commented out some print statements used for debugging.
</commit_message>
<xml_diff>
--- a/ATT.xlsx
+++ b/ATT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="67">
   <si>
     <t>Number</t>
   </si>
@@ -102,7 +102,13 @@
     <t>August 13 2016</t>
   </si>
   <si>
-    <t>mont's pythons</t>
+    <t>August 20 2016</t>
+  </si>
+  <si>
+    <t>August 21 2016</t>
+  </si>
+  <si>
+    <t>monty's pythons</t>
   </si>
   <si>
     <t>PAID</t>
@@ -144,6 +150,15 @@
     <t>04:46 PM</t>
   </si>
   <si>
+    <t>03:53 PM</t>
+  </si>
+  <si>
+    <t>05:49 PM</t>
+  </si>
+  <si>
+    <t>07:08 PM</t>
+  </si>
+  <si>
     <t>darkest coffees</t>
   </si>
   <si>
@@ -159,7 +174,10 @@
     <t>ruby perl</t>
   </si>
   <si>
-    <t>x code</t>
+    <t>05:51 PM</t>
+  </si>
+  <si>
+    <t>x codes</t>
   </si>
   <si>
     <t>04:44 PM</t>
@@ -180,6 +198,12 @@
     <t>03:52 PM</t>
   </si>
   <si>
+    <t>05:50 PM</t>
+  </si>
+  <si>
+    <t>07:10 PM</t>
+  </si>
+  <si>
     <t>node .js</t>
   </si>
   <si>
@@ -192,13 +216,7 @@
     <t>03:05 PM</t>
   </si>
   <si>
-    <t>03:53 PM</t>
-  </si>
-  <si>
-    <t>x codes</t>
-  </si>
-  <si>
-    <t>monty's pythons</t>
+    <t>07:11 PM</t>
   </si>
 </sst>
 </file>
@@ -541,7 +559,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB10"/>
+  <dimension ref="A1:AD10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0" zoomScale="115" zoomScaleNormal="115">
       <selection activeCell="AB10" sqref="AB2:AB10"/>
@@ -557,7 +575,7 @@
     <col bestFit="1" customWidth="1" max="25" min="25" style="1" width="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:30">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -642,16 +660,22 @@
       <c r="AB1" t="s">
         <v>27</v>
       </c>
+      <c r="AC1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:30">
       <c r="A2" s="3" t="n">
         <v>123456789</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D2" s="4" t="n">
         <v>0.411805555555556</v>
@@ -687,51 +711,57 @@
         <v>0.8284722222222222</v>
       </c>
       <c r="O2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="P2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="Q2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="S2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="T2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="U2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="V2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="W2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="X2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="Y2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="AA2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="AB2" t="s">
-        <v>58</v>
+        <v>44</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:30">
       <c r="A3" s="3" t="n">
         <v>543543543</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D3" s="4" t="n">
         <v>0.411805555555556</v>
@@ -767,22 +797,22 @@
         <v>0.536805555555556</v>
       </c>
       <c r="Q3" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="S3" s="4" t="n">
         <v>0.536805555555556</v>
       </c>
       <c r="U3" s="4" t="n"/>
     </row>
-    <row r="4" spans="1:28">
+    <row r="4" spans="1:30">
       <c r="A4" s="3" t="n">
         <v>796448521</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D4" s="4" t="n">
         <v>0.536805555555556</v>
@@ -806,166 +836,187 @@
         <v>0.536805555555556</v>
       </c>
       <c r="S4" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:28">
+    <row r="5" spans="1:30">
       <c r="A5" s="3" t="n">
         <v>741852963</v>
       </c>
       <c r="B5" t="s">
+        <v>51</v>
+      </c>
+      <c r="W5" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD5" t="s">
         <v>46</v>
       </c>
-      <c r="W5" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>41</v>
-      </c>
     </row>
-    <row r="6" spans="1:28">
+    <row r="6" spans="1:30">
       <c r="A6" s="3" t="n">
         <v>604604604</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="X6" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="Y6" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="Z6" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="AA6" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="AB6" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:28">
+    <row r="7" spans="1:30">
       <c r="A7" s="3" t="n">
         <v>789789789</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="X7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:28">
+    <row r="8" spans="1:30">
       <c r="A8" s="3" t="n">
         <v>123123123</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="AA8" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="AB8" t="s">
-        <v>53</v>
+        <v>59</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>60</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:28">
+    <row r="9" spans="1:30">
       <c r="A9" t="n">
         <v>321321321</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="AA9" t="s">
-        <v>55</v>
+        <v>63</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:28">
+    <row r="10" spans="1:30">
       <c r="A10" t="n">
         <v>654654654</v>
       </c>
       <c r="B10" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="E10" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="F10" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="G10" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="H10" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="I10" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="J10" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="K10" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="L10" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="M10" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="N10" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="O10" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="P10" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="Q10" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="R10" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="S10" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="T10" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="U10" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="V10" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="W10" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="X10" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="Y10" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="Z10" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="AA10" t="s">
-        <v>57</v>
+        <v>65</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>60</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>